<commit_message>
Made a few changes to GroupPlan (My Side Only)
</commit_message>
<xml_diff>
--- a/ProjectPlanningDocs/GroupPlan.xlsx
+++ b/ProjectPlanningDocs/GroupPlan.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29F5293A-49C1-4CCD-9BA9-CA34C8B2F003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CamposDev\Workspace-Github\ParkingGarageProject\ProjectPlanningDocs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECFD4B0-28E9-4D7D-9CCF-C7932CAE7DCB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,15 +68,6 @@
     <t>LoginPane</t>
   </si>
   <si>
-    <t>UserInsertPane</t>
-  </si>
-  <si>
-    <t>CheckInPane (Tab Pane?)(tab)</t>
-  </si>
-  <si>
-    <t>CheckOutPane(tab)</t>
-  </si>
-  <si>
     <t>ListViewOpenTickets(gui)</t>
   </si>
   <si>
@@ -127,17 +122,26 @@
     <t>Custom Buttons (CamposButtons)</t>
   </si>
   <si>
-    <t>LightWorkUtil</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;------this number is a blantant lie</t>
+  </si>
+  <si>
+    <t>SignUpPane</t>
+  </si>
+  <si>
+    <t>CheckInPane (Extends TabPane?)</t>
+  </si>
+  <si>
+    <t>CheckOutPane(extends Tab)</t>
+  </si>
+  <si>
+    <t>LightWork</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,22 +521,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="18.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.109375" style="2"/>
+    <col min="8" max="8" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +552,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -560,7 +564,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -572,7 +576,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -584,7 +588,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -596,7 +600,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -608,7 +612,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -620,7 +624,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -632,7 +636,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -644,9 +648,9 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
         <v>60</v>
@@ -656,9 +660,9 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1">
         <v>60</v>
@@ -668,9 +672,9 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1">
         <v>60</v>
@@ -680,23 +684,23 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
         <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>120</v>
@@ -706,45 +710,45 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
         <v>180</v>
@@ -753,26 +757,26 @@
         <v>120</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2">
         <v>90</v>
@@ -781,63 +785,63 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2">
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <v>880</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a Legend to GroupPlan for Work Status'; ;
</commit_message>
<xml_diff>
--- a/ProjectPlanningDocs/GroupPlan.xlsx
+++ b/ProjectPlanningDocs/GroupPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CamposDev\Workspace-Github\ParkingGarageProject\ProjectPlanningDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937A527E-30E4-4A44-A439-D56C7A7542C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D415644-FC38-47F1-87B3-5503C22D99CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,9 +178,21 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="5"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,6 +238,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,6 +259,129 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{555C8174-345D-47AC-BC5D-DC0AF613BB7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6926580" y="304800"/>
+          <a:ext cx="2095500" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" u="sng"/>
+            <a:t>Legend</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Red</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" baseline="0"/>
+            <a:t> = Not Done, heavy work heavy work</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Orange</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" baseline="0"/>
+            <a:t> = Work in Progress</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Green</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" baseline="0"/>
+            <a:t> = Done, light work light work</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -658,7 +799,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1">
@@ -670,7 +811,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="1">
@@ -682,7 +823,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="1">
@@ -694,7 +835,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="1">
@@ -720,7 +861,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="1">
@@ -768,7 +909,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="1">
@@ -842,7 +983,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="2">
@@ -860,5 +1001,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>